<commit_message>
Small changes in footprint and resource allocations
</commit_message>
<xml_diff>
--- a/MRIO/Aggregations/Fossil_Fuels.xlsx
+++ b/MRIO/Aggregations/Fossil_Fuels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\MEAT_SSA\MRIO\Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E493E8-73F4-4A66-A30D-3BA369200F34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3472649-2DC2-4ABE-99B3-C8BB63E084ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="227">
   <si>
     <t>Aggregation</t>
   </si>
@@ -672,9 +672,6 @@
   </si>
   <si>
     <t>Services</t>
-  </si>
-  <si>
-    <t>Transport</t>
   </si>
   <si>
     <t>Waste management</t>
@@ -1111,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1134,10 +1131,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1145,10 +1142,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1156,10 +1153,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1167,10 +1164,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1178,10 +1175,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1189,10 +1186,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1200,10 +1197,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1211,10 +1208,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1222,10 +1219,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1233,10 +1230,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1244,10 +1241,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1255,10 +1252,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1266,10 +1263,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1277,10 +1274,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,10 +1285,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1299,10 +1296,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1310,10 +1307,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1321,10 +1318,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1335,7 +1332,7 @@
         <v>213</v>
       </c>
       <c r="C20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1346,7 +1343,7 @@
         <v>213</v>
       </c>
       <c r="C21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1357,7 +1354,7 @@
         <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1368,7 +1365,7 @@
         <v>213</v>
       </c>
       <c r="C23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1379,7 +1376,7 @@
         <v>213</v>
       </c>
       <c r="C24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1390,7 +1387,7 @@
         <v>213</v>
       </c>
       <c r="C25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1401,7 +1398,7 @@
         <v>213</v>
       </c>
       <c r="C26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1412,7 +1409,7 @@
         <v>213</v>
       </c>
       <c r="C27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1423,7 +1420,7 @@
         <v>213</v>
       </c>
       <c r="C28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,7 +1431,7 @@
         <v>213</v>
       </c>
       <c r="C29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1445,7 +1442,7 @@
         <v>213</v>
       </c>
       <c r="C30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1456,7 +1453,7 @@
         <v>213</v>
       </c>
       <c r="C31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1467,7 +1464,7 @@
         <v>213</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1478,7 +1475,7 @@
         <v>213</v>
       </c>
       <c r="C33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1489,7 +1486,7 @@
         <v>213</v>
       </c>
       <c r="C34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1500,7 +1497,7 @@
         <v>213</v>
       </c>
       <c r="C35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1511,7 +1508,7 @@
         <v>214</v>
       </c>
       <c r="C36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1522,7 +1519,7 @@
         <v>214</v>
       </c>
       <c r="C37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1533,7 +1530,7 @@
         <v>214</v>
       </c>
       <c r="C38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1544,7 +1541,7 @@
         <v>214</v>
       </c>
       <c r="C39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1552,10 +1549,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1563,10 +1560,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1574,10 +1571,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1585,10 +1582,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1596,10 +1593,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1607,10 +1604,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1618,10 +1615,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1629,10 +1626,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1640,10 +1637,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1651,10 +1648,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C49" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1662,10 +1659,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1673,10 +1670,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1684,10 +1681,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1695,10 +1692,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1706,10 +1703,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1717,10 +1714,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1728,10 +1725,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1739,10 +1736,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1750,10 +1747,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1761,10 +1758,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1772,10 +1769,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1783,10 +1780,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1794,10 +1791,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1805,10 +1802,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1816,10 +1813,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C64" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1827,10 +1824,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C65" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1838,10 +1835,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C66" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1849,10 +1846,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C67" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1860,10 +1857,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C68" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1871,10 +1868,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1882,10 +1879,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C70" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1893,10 +1890,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1904,10 +1901,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1915,10 +1912,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1926,10 +1923,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1937,10 +1934,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C75" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1948,10 +1945,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C76" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1959,10 +1956,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1970,10 +1967,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1981,10 +1978,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C79" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1992,10 +1989,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C80" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -2003,10 +2000,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C81" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -2014,10 +2011,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -2025,10 +2022,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C83" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -2036,10 +2033,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C84" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -2047,10 +2044,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C85" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -2058,10 +2055,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C86" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -2069,10 +2066,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C87" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -2080,10 +2077,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C88" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -2091,10 +2088,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -2102,10 +2099,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -2113,10 +2110,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C91" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -2127,7 +2124,7 @@
         <v>215</v>
       </c>
       <c r="C92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -2138,7 +2135,7 @@
         <v>215</v>
       </c>
       <c r="C93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -2146,10 +2143,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C94" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2160,7 +2157,7 @@
         <v>215</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -2168,10 +2165,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -2179,10 +2176,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C97" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -2190,10 +2187,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C98" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -2201,10 +2198,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -2212,10 +2209,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C100" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -2223,10 +2220,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C101" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -2234,10 +2231,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C102" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -2245,10 +2242,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C103" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -2256,10 +2253,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C104" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -2267,10 +2264,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C105" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -2278,10 +2275,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C106" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -2289,10 +2286,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -2300,10 +2297,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C108" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -2314,7 +2311,7 @@
         <v>215</v>
       </c>
       <c r="C109" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -2325,7 +2322,7 @@
         <v>215</v>
       </c>
       <c r="C110" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -2333,10 +2330,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C111" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -2347,7 +2344,7 @@
         <v>215</v>
       </c>
       <c r="C112" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -2355,10 +2352,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -2369,7 +2366,7 @@
         <v>215</v>
       </c>
       <c r="C114" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -2380,7 +2377,7 @@
         <v>215</v>
       </c>
       <c r="C115" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -2388,10 +2385,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C116" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2402,7 +2399,7 @@
         <v>215</v>
       </c>
       <c r="C117" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -2413,7 +2410,7 @@
         <v>215</v>
       </c>
       <c r="C118" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -2424,7 +2421,7 @@
         <v>215</v>
       </c>
       <c r="C119" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -2435,7 +2432,7 @@
         <v>215</v>
       </c>
       <c r="C120" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -2446,7 +2443,7 @@
         <v>215</v>
       </c>
       <c r="C121" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -2454,10 +2451,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C122" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -2465,10 +2462,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C123" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -2476,10 +2473,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C124" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -2487,10 +2484,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C125" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -2498,10 +2495,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C126" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -2509,10 +2506,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C127" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -2523,7 +2520,7 @@
         <v>215</v>
       </c>
       <c r="C128" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -2534,7 +2531,7 @@
         <v>215</v>
       </c>
       <c r="C129" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -2545,7 +2542,7 @@
         <v>215</v>
       </c>
       <c r="C130" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -2556,7 +2553,7 @@
         <v>215</v>
       </c>
       <c r="C131" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -2567,7 +2564,7 @@
         <v>215</v>
       </c>
       <c r="C132" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -2578,7 +2575,7 @@
         <v>215</v>
       </c>
       <c r="C133" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -2589,7 +2586,7 @@
         <v>215</v>
       </c>
       <c r="C134" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -2600,7 +2597,7 @@
         <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -2611,7 +2608,7 @@
         <v>215</v>
       </c>
       <c r="C136" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -2622,7 +2619,7 @@
         <v>215</v>
       </c>
       <c r="C137" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -2633,7 +2630,7 @@
         <v>215</v>
       </c>
       <c r="C138" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -2644,7 +2641,7 @@
         <v>215</v>
       </c>
       <c r="C139" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -2655,7 +2652,7 @@
         <v>215</v>
       </c>
       <c r="C140" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -2663,10 +2660,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C141" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -2674,10 +2671,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C142" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -2685,10 +2682,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C143" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -2696,10 +2693,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C144" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -2707,10 +2704,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C145" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -2718,10 +2715,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C146" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2729,10 +2726,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C147" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -2740,10 +2737,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C148" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -2751,10 +2748,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C149" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -2762,10 +2759,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C150" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -2773,10 +2770,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C151" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -2784,10 +2781,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C152" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -2795,10 +2792,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C153" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -2806,10 +2803,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C154" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -2817,10 +2814,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C155" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -2828,10 +2825,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C156" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -2839,10 +2836,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C157" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -2850,10 +2847,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C158" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -2861,10 +2858,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C159" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -2872,10 +2869,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C160" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -2886,7 +2883,7 @@
         <v>215</v>
       </c>
       <c r="C161" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -2897,7 +2894,7 @@
         <v>215</v>
       </c>
       <c r="C162" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -2908,7 +2905,7 @@
         <v>215</v>
       </c>
       <c r="C163" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -2919,7 +2916,7 @@
         <v>215</v>
       </c>
       <c r="C164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -2930,7 +2927,7 @@
         <v>215</v>
       </c>
       <c r="C165" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2958,7 +2955,7 @@
         <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2966,7 +2963,7 @@
         <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2974,7 +2971,7 @@
         <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2982,7 +2979,7 @@
         <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2990,7 +2987,7 @@
         <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2998,7 +2995,7 @@
         <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3006,7 +3003,7 @@
         <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3014,7 +3011,7 @@
         <v>172</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3022,7 +3019,7 @@
         <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3030,7 +3027,7 @@
         <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -3038,7 +3035,7 @@
         <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3046,7 +3043,7 @@
         <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -3054,7 +3051,7 @@
         <v>177</v>
       </c>
       <c r="B14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3062,7 +3059,7 @@
         <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3070,7 +3067,7 @@
         <v>179</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3078,7 +3075,7 @@
         <v>180</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3086,7 +3083,7 @@
         <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3094,7 +3091,7 @@
         <v>182</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3102,7 +3099,7 @@
         <v>183</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3110,7 +3107,7 @@
         <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -3118,7 +3115,7 @@
         <v>185</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3126,7 +3123,7 @@
         <v>186</v>
       </c>
       <c r="B23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -3134,7 +3131,7 @@
         <v>187</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3142,7 +3139,7 @@
         <v>188</v>
       </c>
       <c r="B25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -3150,7 +3147,7 @@
         <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -3158,7 +3155,7 @@
         <v>190</v>
       </c>
       <c r="B27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -3166,7 +3163,7 @@
         <v>191</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -3174,7 +3171,7 @@
         <v>192</v>
       </c>
       <c r="B29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -3182,7 +3179,7 @@
         <v>193</v>
       </c>
       <c r="B30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -3190,7 +3187,7 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -3198,7 +3195,7 @@
         <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3206,7 +3203,7 @@
         <v>196</v>
       </c>
       <c r="B33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -3214,7 +3211,7 @@
         <v>197</v>
       </c>
       <c r="B34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -3222,7 +3219,7 @@
         <v>198</v>
       </c>
       <c r="B35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -3230,7 +3227,7 @@
         <v>199</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3238,7 +3235,7 @@
         <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -3246,7 +3243,7 @@
         <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -3254,7 +3251,7 @@
         <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -3262,7 +3259,7 @@
         <v>203</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3270,7 +3267,7 @@
         <v>204</v>
       </c>
       <c r="B41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -3278,7 +3275,7 @@
         <v>205</v>
       </c>
       <c r="B42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -3286,7 +3283,7 @@
         <v>206</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -3294,7 +3291,7 @@
         <v>207</v>
       </c>
       <c r="B44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -3302,7 +3299,7 @@
         <v>208</v>
       </c>
       <c r="B45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -3310,7 +3307,7 @@
         <v>209</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -3318,7 +3315,7 @@
         <v>210</v>
       </c>
       <c r="B47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -3326,7 +3323,7 @@
         <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -3334,7 +3331,7 @@
         <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>